<commit_message>
finish tenant and deploy
</commit_message>
<xml_diff>
--- a/seeds/schemas/tenant_accounts_1.xlsx
+++ b/seeds/schemas/tenant_accounts_1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="columns_mapper" sheetId="1" state="visible" r:id="rId3"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="81">
   <si>
     <t xml:space="preserve">key</t>
   </si>
@@ -98,40 +98,34 @@
     <t xml:space="preserve">tenant moderator role</t>
   </si>
   <si>
-    <t xml:space="preserve">TenantFind|TenantList|TenantUpdate|PageCreate|PageFind|PageList|PageUpdate|SectionCreate|SectionFind|SectionList|SectionUpdate</t>
+    <t xml:space="preserve">TenantFind|TenantList|TenantUpdate|PageFind|PageList|PageUpdate|SectionFind|SectionList|SectionUpdate|PartialList|PartialCreate|PartialUpdate|PartialDelete|PartialDeleteRestore|ObjectList|ObjectCreate|ObjectDelete</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tech Innovators</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user_type </t>
+  </si>
+  <si>
+    <t xml:space="preserve">user_phone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user_email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user_password#</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hassan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hassan@devkit.com</t>
   </si>
   <si>
     <t xml:space="preserve">ABC Hotels</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tech  moderator</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TenantFind|TenantList|TenantUpdate|PageFind|PageList|PageUpdate|SectionFind|SectionList|SectionUpdate|PartialList|PartialCreate|PartialUpdate|PartialDelete|PartialDeleteRestore</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tech Innovators</t>
-  </si>
-  <si>
-    <t xml:space="preserve">user_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">user_type </t>
-  </si>
-  <si>
-    <t xml:space="preserve">user_phone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">user_email</t>
-  </si>
-  <si>
-    <t xml:space="preserve">user_password#</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hassan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hassan@devkit.com</t>
   </si>
   <si>
     <t xml:space="preserve">rashad</t>
@@ -703,7 +697,7 @@
       <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="95.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="98.16"/>
@@ -797,13 +791,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="77.515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="77.515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
@@ -822,7 +816,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="39" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
         <v>21</v>
       </c>
@@ -832,33 +826,19 @@
       <c r="C2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E2" s="1" t="n">
         <v>10</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E3" s="1" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="1"/>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -877,27 +857,27 @@
   </sheetPr>
   <dimension ref="A1:H1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="77.515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="77.515625" defaultRowHeight="13.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>10</v>
@@ -909,7 +889,7 @@
     </row>
     <row r="2" customFormat="false" ht="15.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>14</v>
@@ -918,7 +898,7 @@
         <v>1020002001</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E2" s="2" t="n">
         <v>123456</v>
@@ -927,12 +907,12 @@
         <v>21</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>14</v>
@@ -941,16 +921,16 @@
         <v>1020002002</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E3" s="2" t="n">
         <v>123456</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -982,14 +962,14 @@
       <selection pane="topLeft" activeCell="C40" activeCellId="0" sqref="C40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.81"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>14</v>
@@ -997,18 +977,18 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1029,11 +1009,11 @@
   </sheetPr>
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="18.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="9"/>
@@ -1046,16 +1026,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>41</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>43</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>4</v>
@@ -1069,255 +1049,255 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="D2" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="E2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="D3" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>52</v>
-      </c>
       <c r="E3" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="D4" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="E4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="D5" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="E5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>66</v>
-      </c>
       <c r="E6" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="19.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="E7" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="27.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="27.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="27.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="39.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B11" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="52.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="7" t="s">
+      <c r="C11" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="D11" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="E11" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="B12" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="27.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>82</v>
-      </c>
       <c r="C12" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
add abc hotels sample data
</commit_message>
<xml_diff>
--- a/seeds/schemas/tenant_accounts_1.xlsx
+++ b/seeds/schemas/tenant_accounts_1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="columns_mapper" sheetId="1" state="visible" r:id="rId3"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="78">
   <si>
     <t xml:space="preserve">key</t>
   </si>
@@ -240,52 +240,11 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">gallery</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Gallery</t>
-  </si>
-  <si>
-    <t xml:space="preserve">الاستوديو</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/gallery</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">06_</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="CommitMono Nerd Font"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">header_</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
       <t xml:space="preserve">contact</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Contact</t>
+    <t xml:space="preserve">Contact Us</t>
   </si>
   <si>
     <t xml:space="preserve">اتصل بنا</t>
@@ -306,6 +265,12 @@
     <t xml:space="preserve">Our Gallery</t>
   </si>
   <si>
+    <t xml:space="preserve">الاستوديو</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/gallery</t>
+  </si>
+  <si>
     <t xml:space="preserve">03_footer_services</t>
   </si>
   <si>
@@ -325,9 +290,6 @@
   </si>
   <si>
     <t xml:space="preserve">05_footer_contact_us</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contact Us</t>
   </si>
 </sst>
 </file>
@@ -694,7 +656,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+      <selection pane="topLeft" activeCell="B11" activeCellId="1" sqref="C13:C14 B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -793,8 +755,8 @@
   </sheetPr>
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B11" activeCellId="1" sqref="C13:C14 B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="77.515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -816,7 +778,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="39" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
         <v>21</v>
       </c>
@@ -858,7 +820,7 @@
   <dimension ref="A1:H1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="C13:C14 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="77.515625" defaultRowHeight="13.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -959,7 +921,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C40" activeCellId="0" sqref="C40"/>
+      <selection pane="topLeft" activeCell="C40" activeCellId="1" sqref="C13:C14 C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1007,10 +969,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C13:C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1139,7 +1101,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="19.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
         <v>61</v>
       </c>
@@ -1162,21 +1124,21 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="19.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
+    <row r="7" customFormat="false" ht="27.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>36</v>
+        <v>49</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>32</v>
@@ -1187,16 +1149,16 @@
     </row>
     <row r="8" customFormat="false" ht="27.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="D8" s="7" t="s">
         <v>70</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>50</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>37</v>
@@ -1216,10 +1178,10 @@
         <v>72</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>37</v>
@@ -1231,7 +1193,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="27.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="39.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="7" t="s">
         <v>73</v>
       </c>
@@ -1239,10 +1201,10 @@
         <v>74</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>59</v>
+        <v>75</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>76</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>37</v>
@@ -1254,18 +1216,18 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="39.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="7" t="s">
-        <v>75</v>
+    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="s">
+        <v>77</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>37</v>
@@ -1277,31 +1239,11 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>46</v>
-      </c>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C14" s="4"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C15" s="4"/>
+      <c r="C15" s="8"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="8"/>
@@ -1312,9 +1254,7 @@
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C18" s="8"/>
     </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C19" s="8"/>
-    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <autoFilter ref="A1:D3"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>